<commit_message>
worked on BOM (also got approval for layout!)
</commit_message>
<xml_diff>
--- a/Documentation/BOM Documents/BMS_2021_BOM.xlsx
+++ b/Documentation/BOM Documents/BMS_2021_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\GitHub\BMS_Hardware\Documentation\BOM Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E61D6F8-BA9C-4662-AEFC-29F1BEAA4EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291B4CBC-E227-4107-8BD2-AAF0494D811C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8655" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="MRDT BOM Template.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId4" roundtripDataSignature="AMtx7mjKPurHDp02zZJuDnSmJ/SMEm6ufw=="/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="147">
   <si>
     <t>Id</t>
   </si>
@@ -129,9 +130,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>D26,D25,D24,D23,D22,D21</t>
-  </si>
-  <si>
     <t>D20,D18,D17,D6,D7,D8,D9,D10,D13,D14,D15</t>
   </si>
   <si>
@@ -409,6 +407,66 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-078M2L/726831</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>Blue LED</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>D26,D25,D22,D21</t>
+  </si>
+  <si>
+    <t>Greed LED</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=WM4801-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex-llc/0705430042/WM4830-ND/313745</t>
+  </si>
+  <si>
+    <t>FanConn  (08-PCB Vertical)</t>
+  </si>
+  <si>
+    <t>TempConn and LCD_Conn(03-PCB Vertical)</t>
+  </si>
+  <si>
+    <t>cellFilterConn (09-PCB Vertical)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex-llc/0705430043/WM4831-ND/313746</t>
+  </si>
+  <si>
+    <t>ESTOP Mosfets</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex-llc/0705430003/WM4802-ND/114923</t>
+  </si>
+  <si>
+    <t>ON/OFFconn (04-PCB Vertical)</t>
+  </si>
+  <si>
+    <t>ESTOPconn (04-PCB Vertical)</t>
+  </si>
+  <si>
+    <t>TIVA Headers</t>
+  </si>
+  <si>
+    <t>22uF Capacitor</t>
+  </si>
+  <si>
+    <t>Charging Anderson</t>
   </si>
 </sst>
 </file>
@@ -417,9 +475,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -460,6 +518,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -475,7 +541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -532,13 +598,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -579,10 +669,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -904,10 +1011,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -916,8 +1023,8 @@
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="5"/>
-    <col min="6" max="6" width="14.44140625" style="4"/>
+    <col min="5" max="5" width="14.44140625" style="22"/>
+    <col min="6" max="6" width="23.5" style="20" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" style="3"/>
     <col min="8" max="8" width="14.44140625" style="5"/>
     <col min="9" max="9" width="14.44140625" style="4"/>
@@ -942,8 +1049,8 @@
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -981,10 +1088,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -998,10 +1108,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J3" s="2">
         <v>4</v>
@@ -1015,19 +1125,19 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>110</v>
+        <v>72</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="J4" s="2">
         <v>7</v>
       </c>
-      <c r="N4" s="12" t="s">
-        <v>104</v>
+      <c r="N4" s="17" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1038,13 +1148,13 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>112</v>
+        <v>73</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="J5" s="2">
         <v>14</v>
@@ -1052,8 +1162,8 @@
       <c r="K5" s="15">
         <v>0.1</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>127</v>
+      <c r="N5" s="17" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1064,16 +1174,19 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>140</v>
       </c>
       <c r="J6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>106</v>
+      <c r="N6" s="17" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1084,19 +1197,19 @@
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>111</v>
+        <v>75</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>103</v>
+      <c r="N7" s="17" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1107,13 +1220,19 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>143</v>
       </c>
       <c r="J8" s="2">
         <v>1</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1124,13 +1243,19 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="J9" s="2">
         <v>2</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1141,16 +1266,16 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
       </c>
-      <c r="N10" s="12" t="s">
-        <v>107</v>
+      <c r="N10" s="17" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1161,19 +1286,19 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J11" s="2">
         <v>2</v>
       </c>
-      <c r="N11" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="N11" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1181,13 +1306,19 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1198,10 +1329,10 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J13" s="2">
         <v>3</v>
@@ -1215,10 +1346,10 @@
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1232,10 +1363,10 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="2">
         <v>2</v>
@@ -1249,16 +1380,22 @@
         <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="N16" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1266,19 +1403,19 @@
         <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="6">
         <v>330</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>113</v>
+      <c r="F17" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="J17" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1286,19 +1423,19 @@
         <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="6">
         <v>500</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>114</v>
+      <c r="F18" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1306,19 +1443,19 @@
         <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>115</v>
+        <v>84</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>114</v>
       </c>
       <c r="J19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1326,19 +1463,19 @@
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>116</v>
+        <v>85</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>115</v>
       </c>
       <c r="J20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1346,19 +1483,19 @@
         <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>117</v>
+        <v>86</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="J21" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1366,19 +1503,19 @@
         <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>118</v>
+        <v>87</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>117</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1386,307 +1523,342 @@
         <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="J24" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J24" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="3"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="3"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="3"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="3"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F27" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J27" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>119</v>
+        <v>93</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="J30" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="J32" s="2">
         <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="3">
-        <v>26</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J32" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="J33" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="J34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="J35" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="J36" s="2">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="J37" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>121</v>
+        <v>100</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="J38" s="2">
         <v>1</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>122</v>
+        <v>101</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="J39" s="2">
-        <v>1</v>
-      </c>
-      <c r="N39" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="3">
-        <v>34</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="J40" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="3">
-        <v>35</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J41" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="3">
-        <v>36</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="N39" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="J42" s="2">
-        <v>14</v>
-      </c>
-      <c r="K42" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="N42" s="12" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1696,11 +1868,17 @@
     <hyperlink ref="N11" r:id="rId3" xr:uid="{280D3A21-B161-46D5-85E7-806FAB74438A}"/>
     <hyperlink ref="N6" r:id="rId4" xr:uid="{6D616F6E-9D6C-49D3-A300-A49C6F64786E}"/>
     <hyperlink ref="N10" r:id="rId5" xr:uid="{3D3C2A6C-012D-4837-A1CA-8039AE7F8AF1}"/>
-    <hyperlink ref="N38" r:id="rId6" xr:uid="{22D1745B-2792-41E4-AC3D-415F6C32CB33}"/>
-    <hyperlink ref="N39" r:id="rId7" xr:uid="{2FA80049-B2C7-4E06-9AD6-9FB0FF96CF71}"/>
-    <hyperlink ref="N42" r:id="rId8" xr:uid="{33708AC3-0FCB-4F17-8C2D-8505B4F3847D}"/>
+    <hyperlink ref="N35" r:id="rId6" xr:uid="{22D1745B-2792-41E4-AC3D-415F6C32CB33}"/>
+    <hyperlink ref="N36" r:id="rId7" xr:uid="{2FA80049-B2C7-4E06-9AD6-9FB0FF96CF71}"/>
+    <hyperlink ref="N39" r:id="rId8" xr:uid="{33708AC3-0FCB-4F17-8C2D-8505B4F3847D}"/>
     <hyperlink ref="N5" r:id="rId9" xr:uid="{65772F62-786D-40A0-9A7F-D75CBAB19AAC}"/>
+    <hyperlink ref="N28" r:id="rId10" xr:uid="{E878F688-7F7E-4587-9364-E278A92B22C7}"/>
+    <hyperlink ref="N12" r:id="rId11" xr:uid="{FF317A3A-67E6-4251-9A40-76D1B0199826}"/>
+    <hyperlink ref="N9" r:id="rId12" xr:uid="{0A59E2DA-A92B-446D-BCE4-56F3FE4FA316}"/>
+    <hyperlink ref="N8" r:id="rId13" xr:uid="{EA067FD7-EA95-4E53-AB71-E38F5E206ABB}"/>
+    <hyperlink ref="N16" r:id="rId14" xr:uid="{5CEAD036-B3C5-4762-829C-0A1B1C45219C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
silkscreens added to board, BOM continued
added part names and slowly compiling digikey links
</commit_message>
<xml_diff>
--- a/Documentation/BOM Documents/BMS_2021_BOM.xlsx
+++ b/Documentation/BOM Documents/BMS_2021_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\GitHub\BMS_Hardware\Documentation\BOM Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291B4CBC-E227-4107-8BD2-AAF0494D811C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D2CF16-4A88-4E0F-8843-2A367CFF6034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8655" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="150">
   <si>
     <t>Id</t>
   </si>
@@ -67,9 +67,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>REF**,REF**,REF**,REF**</t>
-  </si>
-  <si>
     <t>D4,D11,D12,D1,D2,D3,D5</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>Conn4</t>
   </si>
   <si>
-    <t>V3,V2,V1</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>TM4C129E_Launchpad_FULL_SMD_TOP</t>
   </si>
   <si>
-    <t>4_40_Hole</t>
-  </si>
-  <si>
     <t>RB886CST2RA</t>
   </si>
   <si>
@@ -202,9 +193,6 @@
     <t>MOLEX_SL_08_Vertical</t>
   </si>
   <si>
-    <t>BATT_PWR_VIA</t>
-  </si>
-  <si>
     <t>LT1910_SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.41x3.3mm</t>
   </si>
   <si>
@@ -467,6 +455,27 @@
   </si>
   <si>
     <t>Charging Anderson</t>
+  </si>
+  <si>
+    <t>Logic Switch Mosfet</t>
+  </si>
+  <si>
+    <t>Fan/Buzz Control Mosfet</t>
+  </si>
+  <si>
+    <t>ESTOP High-Side Mosfet Driver</t>
+  </si>
+  <si>
+    <t>Cell Filters Op-Amp</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TL3474ID/550707</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/allegro-microsystems/ACS759ECB-200B-PFF-T/3131286?s=N4IgTCBcDaIIIGEDKB2ArATgKIIEIFowAGIggBQDEL8AVEAXQF8g</t>
+  </si>
+  <si>
+    <t>Current Sensor Hall Effect</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1020,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1088,13 +1097,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -1108,13 +1117,19 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="J3" s="2">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1125,19 +1140,22 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J4" s="2">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0.1</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1148,22 +1166,19 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="J5" s="2">
-        <v>14</v>
-      </c>
-      <c r="K5" s="15">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1174,19 +1189,19 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="J6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1197,19 +1212,19 @@
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="N7" s="17" t="s">
-        <v>102</v>
+      <c r="N7" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1220,19 +1235,19 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>141</v>
+        <v>2</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1243,19 +1258,19 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="J9" s="2">
-        <v>2</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>139</v>
+        <v>1</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1266,19 +1281,22 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="J10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1286,19 +1304,22 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="J11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1306,19 +1327,16 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>136</v>
+        <v>77</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>145</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1329,13 +1347,19 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>78</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>146</v>
       </c>
       <c r="J13" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1346,13 +1370,19 @@
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1363,13 +1393,16 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
+      </c>
+      <c r="D15" s="6">
+        <v>330</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="J15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1380,19 +1413,16 @@
         <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>47</v>
+      </c>
+      <c r="D16" s="6">
+        <v>500</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1403,16 +1433,16 @@
         <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="6">
-        <v>330</v>
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J17" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1423,16 +1453,16 @@
         <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="6">
-        <v>500</v>
+        <v>47</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1443,16 +1473,16 @@
         <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J19" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1463,16 +1493,16 @@
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1483,16 +1513,16 @@
         <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="J21" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1500,19 +1530,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="J22" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1520,16 +1550,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
@@ -1540,19 +1567,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J24" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1560,33 +1584,42 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="J25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
+      <c r="N26" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="J26" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1597,19 +1630,19 @@
         <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="J27" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1617,19 +1650,16 @@
         <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>137</v>
+        <v>89</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="J28" s="2">
-        <v>2</v>
-      </c>
-      <c r="N28" s="19" t="s">
-        <v>134</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1640,16 +1670,19 @@
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J29" s="2">
         <v>1</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1660,16 +1693,16 @@
         <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="J30" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1680,13 +1713,16 @@
         <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>106</v>
       </c>
       <c r="J31" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1697,13 +1733,13 @@
         <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="J32" s="2">
         <v>2</v>
@@ -1717,16 +1753,19 @@
         <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="J33" s="2">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1737,16 +1776,19 @@
         <v>41</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J34" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1757,19 +1799,16 @@
         <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J35" s="2">
-        <v>1</v>
-      </c>
-      <c r="N35" s="17" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1780,19 +1819,16 @@
         <v>43</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1803,82 +1839,44 @@
         <v>44</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J37" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="3">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="3">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="J39" s="2">
         <v>14</v>
       </c>
-      <c r="K39" s="15">
+      <c r="K37" s="15">
         <v>0.1</v>
       </c>
-      <c r="N39" s="17" t="s">
-        <v>125</v>
+      <c r="N37" s="17" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N7" r:id="rId1" xr:uid="{A303DDAB-26E5-43C3-8E37-4539937A62B0}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{6CD3D467-BCCB-4E49-AAE3-EFE375509F35}"/>
-    <hyperlink ref="N11" r:id="rId3" xr:uid="{280D3A21-B161-46D5-85E7-806FAB74438A}"/>
-    <hyperlink ref="N6" r:id="rId4" xr:uid="{6D616F6E-9D6C-49D3-A300-A49C6F64786E}"/>
-    <hyperlink ref="N10" r:id="rId5" xr:uid="{3D3C2A6C-012D-4837-A1CA-8039AE7F8AF1}"/>
-    <hyperlink ref="N35" r:id="rId6" xr:uid="{22D1745B-2792-41E4-AC3D-415F6C32CB33}"/>
-    <hyperlink ref="N36" r:id="rId7" xr:uid="{2FA80049-B2C7-4E06-9AD6-9FB0FF96CF71}"/>
-    <hyperlink ref="N39" r:id="rId8" xr:uid="{33708AC3-0FCB-4F17-8C2D-8505B4F3847D}"/>
-    <hyperlink ref="N5" r:id="rId9" xr:uid="{65772F62-786D-40A0-9A7F-D75CBAB19AAC}"/>
-    <hyperlink ref="N28" r:id="rId10" xr:uid="{E878F688-7F7E-4587-9364-E278A92B22C7}"/>
-    <hyperlink ref="N12" r:id="rId11" xr:uid="{FF317A3A-67E6-4251-9A40-76D1B0199826}"/>
-    <hyperlink ref="N9" r:id="rId12" xr:uid="{0A59E2DA-A92B-446D-BCE4-56F3FE4FA316}"/>
-    <hyperlink ref="N8" r:id="rId13" xr:uid="{EA067FD7-EA95-4E53-AB71-E38F5E206ABB}"/>
-    <hyperlink ref="N16" r:id="rId14" xr:uid="{5CEAD036-B3C5-4762-829C-0A1B1C45219C}"/>
+    <hyperlink ref="N6" r:id="rId1" xr:uid="{A303DDAB-26E5-43C3-8E37-4539937A62B0}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{6CD3D467-BCCB-4E49-AAE3-EFE375509F35}"/>
+    <hyperlink ref="N10" r:id="rId3" xr:uid="{280D3A21-B161-46D5-85E7-806FAB74438A}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{6D616F6E-9D6C-49D3-A300-A49C6F64786E}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{3D3C2A6C-012D-4837-A1CA-8039AE7F8AF1}"/>
+    <hyperlink ref="N33" r:id="rId6" xr:uid="{22D1745B-2792-41E4-AC3D-415F6C32CB33}"/>
+    <hyperlink ref="N34" r:id="rId7" xr:uid="{2FA80049-B2C7-4E06-9AD6-9FB0FF96CF71}"/>
+    <hyperlink ref="N37" r:id="rId8" xr:uid="{33708AC3-0FCB-4F17-8C2D-8505B4F3847D}"/>
+    <hyperlink ref="N4" r:id="rId9" xr:uid="{65772F62-786D-40A0-9A7F-D75CBAB19AAC}"/>
+    <hyperlink ref="N26" r:id="rId10" xr:uid="{E878F688-7F7E-4587-9364-E278A92B22C7}"/>
+    <hyperlink ref="N11" r:id="rId11" xr:uid="{FF317A3A-67E6-4251-9A40-76D1B0199826}"/>
+    <hyperlink ref="N8" r:id="rId12" xr:uid="{0A59E2DA-A92B-446D-BCE4-56F3FE4FA316}"/>
+    <hyperlink ref="N7" r:id="rId13" xr:uid="{EA067FD7-EA95-4E53-AB71-E38F5E206ABB}"/>
+    <hyperlink ref="N14" r:id="rId14" xr:uid="{5CEAD036-B3C5-4762-829C-0A1B1C45219C}"/>
+    <hyperlink ref="N13" r:id="rId15" xr:uid="{9A2E520D-E673-4348-842B-689E947F366B}"/>
+    <hyperlink ref="N29" r:id="rId16" xr:uid="{4A05AF95-B945-4C74-9C9E-BA6B64A12B27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
needed to change R45,R40 ( and the associated other resistor values) to something in stock
Instead of an exact 3.3 V output, now there is 3.287
</commit_message>
<xml_diff>
--- a/Documentation/BOM Documents/BMS_2021_BOM.xlsx
+++ b/Documentation/BOM Documents/BMS_2021_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\GitHub\BMS_Hardware\Documentation\BOM Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D2CF16-4A88-4E0F-8843-2A367CFF6034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33F2217-1F24-4F73-B525-9D48B2E2B46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8655" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="180">
   <si>
     <t>Id</t>
   </si>
@@ -403,18 +403,12 @@
     <t>Blue LED</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t>D24</t>
   </si>
   <si>
     <t>D26,D25,D22,D21</t>
   </si>
   <si>
-    <t>Greed LED</t>
-  </si>
-  <si>
     <t>Fuse</t>
   </si>
   <si>
@@ -476,6 +470,102 @@
   </si>
   <si>
     <t>Current Sensor Hall Effect</t>
+  </si>
+  <si>
+    <t>S5680-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/NPTC102KFMS-RC/776139</t>
+  </si>
+  <si>
+    <t>Only 1 tiva, but 4 headers are needed</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>846-RB886CST2RTR-ND</t>
+  </si>
+  <si>
+    <t>311-8.2MGRTR-ND</t>
+  </si>
+  <si>
+    <t>IRFS7530TRL7PPTR-ND</t>
+  </si>
+  <si>
+    <t>493-5915-1-ND</t>
+  </si>
+  <si>
+    <t>WM4802-ND</t>
+  </si>
+  <si>
+    <t>WM4831-ND</t>
+  </si>
+  <si>
+    <t>2N7002NTR-ND</t>
+  </si>
+  <si>
+    <t>1727-4793-2-ND</t>
+  </si>
+  <si>
+    <t>WM4830-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LT1910ES8-TRPBF/958723</t>
+  </si>
+  <si>
+    <t>LT1910ES8#TRPBFTR-ND</t>
+  </si>
+  <si>
+    <t>296-14407-5-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RT0603DRE07330RL/1074799</t>
+  </si>
+  <si>
+    <t>311-2540-2-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/delta-electronics-cyntec/RLT0816-2-R500-FNH/9762149</t>
+  </si>
+  <si>
+    <t>2037-RLT0816-2-R500-FNHTR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/ESR03EZPF1002/RHM10KADCT-ND/1983753</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTST-C191KGKT/160-1446-1-ND/386834</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTST-C191TBKT/160-1647-1-ND/573587</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTST-C191KRKT/160-1447-1-ND/386836</t>
+  </si>
+  <si>
+    <t>160-1447-1-ND</t>
+  </si>
+  <si>
+    <t>160-1446-1-ND</t>
+  </si>
+  <si>
+    <t>160-1647-1-ND</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/Semiconductors/Discrete-Semiconductors/Diodes-Rectifiers/Zener-Diodes/_/N-ax1mh?P=1yuq69lZ1yzvlkx</t>
+  </si>
+  <si>
+    <t>821-TSZU52C3V3RGG</t>
+  </si>
+  <si>
+    <t>Mouser</t>
   </si>
 </sst>
 </file>
@@ -486,7 +576,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -531,6 +621,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -637,7 +734,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -672,9 +769,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -684,7 +778,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -701,6 +794,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1022,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1032,17 +1130,18 @@
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="22"/>
-    <col min="6" max="6" width="23.5" style="20" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="3"/>
+    <col min="5" max="5" width="14.44140625" style="20"/>
+    <col min="6" max="6" width="23.5" style="18" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" style="6" customWidth="1"/>
     <col min="8" max="8" width="14.44140625" style="5"/>
     <col min="9" max="9" width="14.44140625" style="4"/>
     <col min="10" max="10" width="14.44140625" style="1"/>
-    <col min="11" max="11" width="14.44140625" style="15"/>
+    <col min="11" max="11" width="14.44140625" style="14"/>
     <col min="12" max="12" width="14.44140625" style="5"/>
     <col min="13" max="13" width="14.44140625" style="4"/>
-    <col min="14" max="14" width="47.94140625" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="14.44140625" style="1"/>
+    <col min="14" max="14" width="47.94140625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="23.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="14.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1058,11 +1157,11 @@
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="21" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="9"/>
@@ -1072,7 +1171,7 @@
       <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="9"/>
@@ -1102,11 +1201,26 @@
       <c r="D2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>140</v>
+      <c r="F2" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J2" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="K2" s="14">
+        <v>2.13</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1122,13 +1236,22 @@
       <c r="D3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>105</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J3" s="2">
         <v>7</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="K3" s="14">
+        <v>0.42</v>
+      </c>
+      <c r="N3" s="15" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1145,16 +1268,22 @@
       <c r="D4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="18" t="s">
         <v>107</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J4" s="2">
         <v>14</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="14">
         <v>0.1</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="15" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1171,13 +1300,22 @@
       <c r="D5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>136</v>
+      <c r="F5" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="K5" s="14">
+        <v>2.83</v>
+      </c>
+      <c r="N5" s="15" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1194,17 +1332,26 @@
       <c r="D6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="18" t="s">
         <v>106</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="K6" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="N6" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1217,14 +1364,23 @@
       <c r="D7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>139</v>
+      <c r="F7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>137</v>
+      <c r="K7" s="14">
+        <v>0.82</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1240,14 +1396,23 @@
       <c r="D8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>134</v>
+      <c r="F8" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J8" s="2">
         <v>2</v>
       </c>
-      <c r="N8" s="12" t="s">
-        <v>135</v>
+      <c r="K8" s="14">
+        <v>1.41</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1263,13 +1428,22 @@
       <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>143</v>
+      <c r="F9" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="K9" s="14">
+        <v>0.32</v>
+      </c>
+      <c r="N9" s="15" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1286,13 +1460,22 @@
       <c r="D10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>144</v>
+      <c r="F10" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J10" s="2">
         <v>2</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="K10" s="14">
+        <v>0.24</v>
+      </c>
+      <c r="N10" s="15" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1309,14 +1492,23 @@
       <c r="D11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>132</v>
+      <c r="F11" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J11" s="2">
         <v>1</v>
       </c>
-      <c r="N11" s="17" t="s">
-        <v>131</v>
+      <c r="K11" s="14">
+        <v>1.44</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1332,11 +1524,23 @@
       <c r="D12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>145</v>
+      <c r="F12" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
+      </c>
+      <c r="K12" s="14">
+        <v>5.25</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1352,17 +1556,26 @@
       <c r="D13" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>146</v>
+      <c r="F13" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J13" s="2">
         <v>2</v>
       </c>
-      <c r="N13" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K13" s="14">
+        <v>1.19</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1375,14 +1588,23 @@
       <c r="D14" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="20" t="s">
-        <v>138</v>
+      <c r="F14" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
-      <c r="N14" s="16" t="s">
-        <v>137</v>
+      <c r="K14" s="14">
+        <v>0.82</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1398,11 +1620,23 @@
       <c r="D15" s="6">
         <v>330</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="18" t="s">
         <v>108</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J15" s="2">
         <v>5</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1418,11 +1652,23 @@
       <c r="D16" s="6">
         <v>500</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="18" t="s">
         <v>109</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
+      </c>
+      <c r="K16" s="14">
+        <v>0.53</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1438,8 +1684,11 @@
       <c r="D17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="18" t="s">
         <v>110</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J17" s="2">
         <v>2</v>
@@ -1458,8 +1707,11 @@
       <c r="D18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="18" t="s">
         <v>111</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J18" s="2">
         <v>2</v>
@@ -1478,11 +1730,17 @@
       <c r="D19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="18" t="s">
         <v>112</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J19" s="2">
         <v>6</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1498,8 +1756,11 @@
       <c r="D20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="18" t="s">
         <v>113</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -1518,19 +1779,22 @@
       <c r="D21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="20" t="s">
-        <v>129</v>
+      <c r="F21" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>58</v>
@@ -1538,14 +1802,26 @@
       <c r="D22" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>128</v>
+      <c r="F22" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J22" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K22" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1555,31 +1831,55 @@
       <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="18" t="s">
         <v>124</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K23" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="20" t="s">
-        <v>125</v>
+      <c r="F24" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K24" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1592,11 +1892,23 @@
       <c r="D25" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="18" t="s">
         <v>114</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J25" s="2">
         <v>11</v>
+      </c>
+      <c r="K25" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1612,14 +1924,17 @@
       <c r="D26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="18" t="s">
-        <v>133</v>
+      <c r="F26" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J26" s="2">
         <v>2</v>
       </c>
-      <c r="N26" s="19" t="s">
-        <v>130</v>
+      <c r="N26" s="17" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1635,8 +1950,11 @@
       <c r="D27" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="20" t="s">
-        <v>142</v>
+      <c r="F27" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J27" s="2">
         <v>1</v>
@@ -1655,8 +1973,11 @@
       <c r="D28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="18" t="s">
         <v>89</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J28" s="2">
         <v>1</v>
@@ -1675,14 +1996,17 @@
       <c r="D29" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="20" t="s">
-        <v>149</v>
+      <c r="F29" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J29" s="2">
         <v>1</v>
       </c>
-      <c r="N29" s="12" t="s">
-        <v>148</v>
+      <c r="N29" s="15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -1698,8 +2022,11 @@
       <c r="D30" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="20" t="s">
-        <v>141</v>
+      <c r="F30" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J30" s="2">
         <v>2</v>
@@ -1718,8 +2045,11 @@
       <c r="D31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="18" t="s">
         <v>106</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J31" s="2">
         <v>8</v>
@@ -1738,8 +2068,11 @@
       <c r="D32" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="18" t="s">
         <v>115</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J32" s="2">
         <v>2</v>
@@ -1758,13 +2091,16 @@
       <c r="D33" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="18" t="s">
         <v>116</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J33" s="2">
         <v>1</v>
       </c>
-      <c r="N33" s="17" t="s">
+      <c r="N33" s="15" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1781,13 +2117,16 @@
       <c r="D34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="18" t="s">
         <v>117</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J34" s="2">
         <v>1</v>
       </c>
-      <c r="N34" s="17" t="s">
+      <c r="N34" s="15" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1804,8 +2143,11 @@
       <c r="D35" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="18" t="s">
         <v>118</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J35" s="2">
         <v>8</v>
@@ -1824,8 +2166,11 @@
       <c r="D36" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="18" t="s">
         <v>119</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
@@ -1844,16 +2189,19 @@
       <c r="D37" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="18" t="s">
         <v>120</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J37" s="2">
         <v>14</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="14">
         <v>0.1</v>
       </c>
-      <c r="N37" s="17" t="s">
+      <c r="N37" s="15" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1875,8 +2223,15 @@
     <hyperlink ref="N14" r:id="rId14" xr:uid="{5CEAD036-B3C5-4762-829C-0A1B1C45219C}"/>
     <hyperlink ref="N13" r:id="rId15" xr:uid="{9A2E520D-E673-4348-842B-689E947F366B}"/>
     <hyperlink ref="N29" r:id="rId16" xr:uid="{4A05AF95-B945-4C74-9C9E-BA6B64A12B27}"/>
+    <hyperlink ref="N2" r:id="rId17" xr:uid="{11774C2F-92A1-43C5-BE94-8CC93099A65F}"/>
+    <hyperlink ref="N12" r:id="rId18" xr:uid="{283C8578-4905-4530-A2A1-48437A1F7C6A}"/>
+    <hyperlink ref="N15" r:id="rId19" xr:uid="{2D86C145-D066-44A3-82CA-AFDC7BA7FF5C}"/>
+    <hyperlink ref="N19" r:id="rId20" xr:uid="{6798D022-33E4-4EF3-AB00-7E730161CCC1}"/>
+    <hyperlink ref="N23" r:id="rId21" xr:uid="{920F633D-78BA-4504-BB06-0838F2B2C0A0}"/>
+    <hyperlink ref="N22" r:id="rId22" xr:uid="{8D8F45CF-6DE2-41B4-99D7-A7B0398085AD}"/>
+    <hyperlink ref="N24" r:id="rId23" xr:uid="{7BE41CFB-DF80-4BA5-B8D8-8C94B894C3ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>